<commit_message>
Fix bug in which an invalid table did not generate an error message and end execution of CombatModelerWindow.run_simulation() method. Fix bug in table Lurker Ambushing Action that was causing failures.
</commit_message>
<xml_diff>
--- a/data/combat-tables.xlsx
+++ b/data/combat-tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Users\valen\Documents\Valen\python\python-repository\combat-modeler\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{174B7530-FE84-483B-8387-F84A1DB9DE87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B83D93B8-7F93-4D62-84D6-86753FDC2543}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31620" yWindow="1230" windowWidth="21600" windowHeight="11295" firstSheet="15" activeTab="17" xr2:uid="{E3A1E28D-E878-4C5D-852F-DF902928C313}"/>
+    <workbookView xWindow="32325" yWindow="1395" windowWidth="21600" windowHeight="11295" firstSheet="12" activeTab="12" xr2:uid="{E3A1E28D-E878-4C5D-852F-DF902928C313}"/>
   </bookViews>
   <sheets>
     <sheet name="Tank Ambushing Action" sheetId="5" r:id="rId1"/>
@@ -329,9 +329,6 @@
     <t>14</t>
   </si>
   <si>
-    <t>18-14</t>
-  </si>
-  <si>
     <t>09-10</t>
   </si>
   <si>
@@ -369,6 +366,9 @@
   </si>
   <si>
     <t>09-16</t>
+  </si>
+  <si>
+    <t>08-14</t>
   </si>
 </sst>
 </file>
@@ -1320,8 +1320,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87AA574E-D37F-49B8-B798-FC18005E1FD6}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1374,7 +1374,7 @@
         <v>31</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>91</v>
+        <v>104</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>6</v>
@@ -1526,7 +1526,7 @@
         <v>53</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>17</v>
@@ -1534,7 +1534,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>30</v>
@@ -1543,7 +1543,7 @@
         <v>30</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>18</v>
@@ -1560,7 +1560,7 @@
         <v>84</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>19</v>
@@ -1685,7 +1685,7 @@
         <v>56</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>7</v>
@@ -1693,7 +1693,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>24</v>
@@ -1953,16 +1953,16 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>6</v>
@@ -1973,10 +1973,10 @@
         <v>61</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>61</v>
@@ -2004,7 +2004,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>60</v>
@@ -2060,7 +2060,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44D45E41-876E-47D0-9C4E-C2966178D8A8}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -2122,10 +2122,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>47</v>
@@ -2139,16 +2139,16 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
Add static method Character.check_series() to verify that the contents of the A, B, C, and D series in combat action tables and combat targeting tables are, in fact, properly sequential with no coverage gaps.
</commit_message>
<xml_diff>
--- a/data/combat-tables.xlsx
+++ b/data/combat-tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Users\valen\Documents\Valen\python\python-repository\combat-modeler\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B83D93B8-7F93-4D62-84D6-86753FDC2543}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84F187DE-B5FE-4390-A50D-2A06D30D176B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32325" yWindow="1395" windowWidth="21600" windowHeight="11295" firstSheet="12" activeTab="12" xr2:uid="{E3A1E28D-E878-4C5D-852F-DF902928C313}"/>
+    <workbookView xWindow="6915" yWindow="870" windowWidth="21600" windowHeight="11295" firstSheet="14" activeTab="16" xr2:uid="{E3A1E28D-E878-4C5D-852F-DF902928C313}"/>
   </bookViews>
   <sheets>
     <sheet name="Tank Ambushing Action" sheetId="5" r:id="rId1"/>
@@ -188,9 +188,6 @@
     <t>02</t>
   </si>
   <si>
-    <t>03-18</t>
-  </si>
-  <si>
     <t>01-20</t>
   </si>
   <si>
@@ -275,9 +272,6 @@
     <t>01-04</t>
   </si>
   <si>
-    <t>12-18</t>
-  </si>
-  <si>
     <t>01-06</t>
   </si>
   <si>
@@ -369,6 +363,12 @@
   </si>
   <si>
     <t>08-14</t>
+  </si>
+  <si>
+    <t>03</t>
+  </si>
+  <si>
+    <t>04-18</t>
   </si>
 </sst>
 </file>
@@ -733,7 +733,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -766,10 +766,10 @@
         <v>36</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>36</v>
+        <v>58</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>5</v>
@@ -946,13 +946,13 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>36</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>26</v>
@@ -972,7 +972,7 @@
         <v>11</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>19</v>
@@ -989,7 +989,7 @@
         <v>11</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>20</v>
@@ -1027,7 +1027,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1057,13 +1057,13 @@
         <v>29</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>26</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>5</v>
@@ -1074,13 +1074,13 @@
         <v>30</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>78</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>80</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>6</v>
@@ -1091,13 +1091,13 @@
         <v>31</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>79</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>81</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>7</v>
@@ -1108,13 +1108,13 @@
         <v>37</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>8</v>
@@ -1122,16 +1122,16 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>9</v>
@@ -1215,7 +1215,7 @@
         <v>21</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>16</v>
@@ -1226,13 +1226,13 @@
         <v>22</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>17</v>
@@ -1240,16 +1240,16 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>83</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>85</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>18</v>
@@ -1257,16 +1257,16 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>19</v>
@@ -1283,7 +1283,7 @@
         <v>13</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>20</v>
@@ -1320,8 +1320,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87AA574E-D37F-49B8-B798-FC18005E1FD6}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1348,16 +1348,16 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>29</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>5</v>
@@ -1365,16 +1365,16 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>31</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>6</v>
@@ -1385,7 +1385,7 @@
         <v>32</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>39</v>
@@ -1399,7 +1399,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>39</v>
@@ -1419,13 +1419,13 @@
         <v>13</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>41</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>9</v>
@@ -1473,7 +1473,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1500,13 +1500,13 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>42</v>
@@ -1517,16 +1517,16 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>17</v>
@@ -1534,7 +1534,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>30</v>
@@ -1543,7 +1543,7 @@
         <v>30</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>18</v>
@@ -1551,16 +1551,16 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>19</v>
@@ -1568,7 +1568,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>71</v>
+        <v>47</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>25</v>
@@ -1577,7 +1577,7 @@
         <v>41</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>20</v>
@@ -1662,13 +1662,13 @@
         <v>22</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>6</v>
@@ -1676,16 +1676,16 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>7</v>
@@ -1693,13 +1693,13 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>24</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>15</v>
@@ -1710,13 +1710,13 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>25</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>25</v>
@@ -1767,7 +1767,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1834,7 +1834,7 @@
         <v>35</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>26</v>
@@ -1845,16 +1845,16 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>60</v>
+        <v>24</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>19</v>
@@ -1871,7 +1871,7 @@
         <v>11</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>20</v>
@@ -1908,8 +1908,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A62B7390-EFCD-45A7-B3D9-980DABF72C1C}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1936,7 +1936,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>21</v>
@@ -1945,7 +1945,7 @@
         <v>21</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>5</v>
@@ -1953,16 +1953,16 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>99</v>
-      </c>
       <c r="C3" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>6</v>
@@ -1970,16 +1970,16 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>7</v>
@@ -1990,10 +1990,10 @@
         <v>39</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>39</v>
@@ -2004,16 +2004,16 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>9</v>
@@ -2097,7 +2097,7 @@
         <v>21</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>16</v>
@@ -2111,10 +2111,10 @@
         <v>22</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>17</v>
@@ -2122,13 +2122,13 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>102</v>
-      </c>
       <c r="C4" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>11</v>
@@ -2139,16 +2139,16 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>103</v>
-      </c>
       <c r="C5" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>19</v>
@@ -2484,7 +2484,7 @@
         <v>43</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>11</v>
@@ -2498,10 +2498,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>21</v>
@@ -2515,16 +2515,16 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="D5" s="3" t="s">
         <v>54</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>55</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>8</v>
@@ -2589,7 +2589,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2633,7 +2633,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>43</v>
+        <v>103</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>30</v>
@@ -2650,16 +2650,16 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>44</v>
+        <v>104</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>31</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>46</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>18</v>
@@ -2676,7 +2676,7 @@
         <v>11</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>19</v>
@@ -2693,7 +2693,7 @@
         <v>11</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>20</v>
@@ -2758,7 +2758,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>26</v>
@@ -2778,13 +2778,13 @@
         <v>31</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>40</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>6</v>
@@ -2801,7 +2801,7 @@
         <v>14</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>7</v>
@@ -2818,7 +2818,7 @@
         <v>15</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>8</v>
@@ -2826,10 +2826,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>12</v>
@@ -2950,10 +2950,10 @@
         <v>31</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>18</v>
@@ -2970,7 +2970,7 @@
         <v>24</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>19</v>
@@ -2987,7 +2987,7 @@
         <v>25</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>20</v>
@@ -3025,7 +3025,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3058,7 +3058,7 @@
         <v>26</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>26</v>
@@ -3069,16 +3069,16 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>67</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>68</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>31</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>6</v>
@@ -3177,7 +3177,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3207,7 +3207,7 @@
         <v>33</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>11</v>
@@ -3221,10 +3221,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>11</v>
@@ -3238,7 +3238,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>30</v>
@@ -3247,7 +3247,7 @@
         <v>38</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>18</v>
@@ -3255,16 +3255,16 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>73</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>75</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>19</v>
@@ -3272,7 +3272,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>71</v>
+        <v>47</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>25</v>
@@ -3363,16 +3363,16 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>30</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>6</v>
@@ -3386,7 +3386,7 @@
         <v>11</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>11</v>
@@ -3400,13 +3400,13 @@
         <v>11</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>57</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>58</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>8</v>
@@ -3420,7 +3420,7 @@
         <v>12</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>25</v>

</xml_diff>